<commit_message>
Commit 006 - Wilton
Adicionado arquivos de Links  Uteis, Canvas e Lista de Requisitos
</commit_message>
<xml_diff>
--- a/Lista de Requisitos .xlsx
+++ b/Lista de Requisitos .xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>Número do Requisito</t>
   </si>
@@ -79,52 +79,64 @@
     <t>09FU</t>
   </si>
   <si>
+    <t>Deve ser permitido que o usuário remova uma oferta de doação</t>
+  </si>
+  <si>
+    <t>10FU</t>
+  </si>
+  <si>
+    <t>Deve ser permitido que a instituição remova um pedido de doação</t>
+  </si>
+  <si>
+    <t>11FU</t>
+  </si>
+  <si>
     <t xml:space="preserve">Deve ser permitido avaliar doações  </t>
   </si>
   <si>
-    <t>10FU</t>
+    <t>12FU</t>
   </si>
   <si>
     <t>Deve ser permitido avaliar instituições</t>
   </si>
   <si>
-    <t>11FU</t>
+    <t>13FU</t>
   </si>
   <si>
     <t>Deve ser permitido consultar o histórico de doadores</t>
   </si>
   <si>
-    <t>12FU</t>
+    <t>14FU</t>
   </si>
   <si>
     <t>Deve ser permitido consultar o histórico de doações</t>
   </si>
   <si>
-    <t>13FU</t>
+    <t>15FU</t>
   </si>
   <si>
     <t>Deve ser calculado um índice de confiabilidade com base nas avaliações dos doadores</t>
   </si>
   <si>
-    <t>14FU</t>
+    <t>16FU</t>
   </si>
   <si>
     <t>Deve ser calculado um índice de confiabilidade com base nas avaliações das instituições</t>
   </si>
   <si>
-    <t>15FU</t>
+    <t>17FU</t>
   </si>
   <si>
     <t>Usuários com índice de confiabilidade baixo devem ser bloqueados automaticamente</t>
   </si>
   <si>
-    <t>16FU</t>
+    <t>18FU</t>
   </si>
   <si>
     <t>Instituições com índice de confiabilidade baixo devem ser bloqueadas automaticamente</t>
   </si>
   <si>
-    <t>17NF</t>
+    <t>19NF</t>
   </si>
   <si>
     <t>O sistema deve apresentar uma opção de ajuda para facilitar o usuário a utilizar o sistema</t>
@@ -133,19 +145,19 @@
     <t>Não funcional</t>
   </si>
   <si>
-    <t>18NF</t>
+    <t>20NF</t>
   </si>
   <si>
     <t>O sistema deve ser online</t>
   </si>
   <si>
-    <t>19NF</t>
+    <t>21NF</t>
   </si>
   <si>
     <t>O sistema deve acessível a partir de qualquer navegador</t>
   </si>
   <si>
-    <t>20NF</t>
+    <t>22NF</t>
   </si>
   <si>
     <t>O sistema deve ser acessível a partir de dispositivos móveis</t>
@@ -390,7 +402,7 @@
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -401,7 +413,7 @@
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -412,7 +424,7 @@
       <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -423,7 +435,7 @@
       <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -435,29 +447,29 @@
         <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>39</v>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21">
@@ -467,15 +479,31 @@
       <c r="B21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>39</v>
+      <c r="C21" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="6"/>
+      <c r="A22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="6"/>
+      <c r="A23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="6"/>
@@ -515,6 +543,12 @@
     </row>
     <row r="36">
       <c r="A36" s="6"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="6"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>